<commit_message>
giai thich file excel
</commit_message>
<xml_diff>
--- a/public/MauExcel/MauTaiSan.xlsx
+++ b/public/MauExcel/MauTaiSan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\QuanLyTaiSan\public\MauExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C24BEBF-BC44-4748-BB53-4322A866CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1775FF97-2501-42C2-9770-E5EAE26DC8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D4C916CF-ABD1-483D-A927-A12C85D42622}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D4C916CF-ABD1-483D-A927-A12C85D42622}"/>
   </bookViews>
   <sheets>
     <sheet name="DuLieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="140">
   <si>
     <t>nhom_tai_san</t>
   </si>
@@ -246,9 +246,6 @@
     <t>loai_tai_san</t>
   </si>
   <si>
-    <t>gia_tri_con_lai'] =</t>
-  </si>
-  <si>
     <t>stt</t>
   </si>
   <si>
@@ -256,6 +253,210 @@
   </si>
   <si>
     <t>Máy in</t>
+  </si>
+  <si>
+    <t>1. Đất, 2. Nhà, 3. Vật kiến trúc (Nhập 1,2,3,… theo danh mục nhóm tài sản)</t>
+  </si>
+  <si>
+    <t>Nhập mã loại tài sản theo nhóm tài sản</t>
+  </si>
+  <si>
+    <t>Mã tài sản</t>
+  </si>
+  <si>
+    <t>Tên tài sản</t>
+  </si>
+  <si>
+    <t>Lý do tăng: Đầu tư, Mua sắm, …</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t>Mã bộ phận sử dụng</t>
+  </si>
+  <si>
+    <t>Mã tỉnh thành phố theo danh mục</t>
+  </si>
+  <si>
+    <t>Mã thuyện, quận theo danh mục</t>
+  </si>
+  <si>
+    <t>Mã xã theo danh mục</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Số tầng</t>
+  </si>
+  <si>
+    <t>chiều dài</t>
+  </si>
+  <si>
+    <t>diện tích xây dựng</t>
+  </si>
+  <si>
+    <t>thể tích</t>
+  </si>
+  <si>
+    <t>năm xây dựng</t>
+  </si>
+  <si>
+    <t>nước sản xuất</t>
+  </si>
+  <si>
+    <t>biển kiểm soát</t>
+  </si>
+  <si>
+    <t>nhãn hiệu tài sản</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>số seri</t>
+  </si>
+  <si>
+    <t>số máy</t>
+  </si>
+  <si>
+    <t>tải trọng</t>
+  </si>
+  <si>
+    <t>số chỗ ngồi</t>
+  </si>
+  <si>
+    <t>số cầu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">công suất </t>
+  </si>
+  <si>
+    <t>dung tích xe</t>
+  </si>
+  <si>
+    <t>giấy công nhận đăng ký số</t>
+  </si>
+  <si>
+    <t>ngày đăng ký</t>
+  </si>
+  <si>
+    <t>cơ quan cấp đăng ký</t>
+  </si>
+  <si>
+    <t>nguồn gốc xe</t>
+  </si>
+  <si>
+    <t>màu sơn</t>
+  </si>
+  <si>
+    <t>người sử dụng</t>
+  </si>
+  <si>
+    <t>hình thức bố trí sử dụng</t>
+  </si>
+  <si>
+    <t>chức danh sử dụng</t>
+  </si>
+  <si>
+    <t>quyết định trang cấp</t>
+  </si>
+  <si>
+    <t>ngày quyết định trang cấp</t>
+  </si>
+  <si>
+    <t>dự án</t>
+  </si>
+  <si>
+    <t>1. Đất, 2. Nhà, 3. Xe ô tô, 4. Tài sản trên 500tr, 5. tài sản dưới 500tr</t>
+  </si>
+  <si>
+    <t>thông số kỹ thuật</t>
+  </si>
+  <si>
+    <t>quản lý nhà nước (hoạt động sự nghiệp)</t>
+  </si>
+  <si>
+    <t>HĐSN - Không KD</t>
+  </si>
+  <si>
+    <t>HĐSN - KD</t>
+  </si>
+  <si>
+    <t>HĐSN - LDLK</t>
+  </si>
+  <si>
+    <t>HĐSN - Cho thuê</t>
+  </si>
+  <si>
+    <t>sử dụng khác</t>
+  </si>
+  <si>
+    <t>trạng thái: 0. chưa ghi tăng, 1. đang sử dụng</t>
+  </si>
+  <si>
+    <t>tổng diện tích</t>
+  </si>
+  <si>
+    <t>giá trị đất</t>
+  </si>
+  <si>
+    <t>ngày mua</t>
+  </si>
+  <si>
+    <t>ngày bắt đầu sử dụng</t>
+  </si>
+  <si>
+    <t>ngày ghi tăng</t>
+  </si>
+  <si>
+    <t>năm theo dõi</t>
+  </si>
+  <si>
+    <t>số năm sử dụng</t>
+  </si>
+  <si>
+    <t>tỷ lệ hao mòn</t>
+  </si>
+  <si>
+    <t>HM/KH năm</t>
+  </si>
+  <si>
+    <t>số năm sử dụng còn lại</t>
+  </si>
+  <si>
+    <t>ngày bắt đầu tính hao mòn yyyy-MM-dd, vd 2024-12-30</t>
+  </si>
+  <si>
+    <t>ngày kết thúc hao mòn yyyy-MM-dd v,  2024-12-30</t>
+  </si>
+  <si>
+    <t>hao mòn lũy kế</t>
+  </si>
+  <si>
+    <t>giá trị còn lại</t>
+  </si>
+  <si>
+    <t>mục đích sử dụng: Đất hoạt động sự nghiệp …</t>
+  </si>
+  <si>
+    <t>diện tích để ở</t>
+  </si>
+  <si>
+    <t>dt bỏ trống</t>
+  </si>
+  <si>
+    <t>dt bị lấn chiếm</t>
+  </si>
+  <si>
+    <t>dt sử dụng hỗn hợp</t>
+  </si>
+  <si>
+    <t>mặc định: vpddt</t>
   </si>
 </sst>
 </file>
@@ -672,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA487DE-4DBA-46C1-BAEE-8030A4010D3F}">
   <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -710,7 +911,7 @@
   <sheetData>
     <row r="1" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1137,10 +1338,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -1343,560 +1544,765 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15E2949-BB3D-448C-A15A-293A8837AA3A}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
+      </c>
+      <c r="C68" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>